<commit_message>
fixed new 2019 data to other survival range
</commit_message>
<xml_diff>
--- a/data/2019 Naeem-Esf, Pro, food/2_days.xlsx
+++ b/data/2019 Naeem-Esf, Pro, food/2_days.xlsx
@@ -466,10 +466,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="5">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="C2" s="5">
-        <v>93.3333333333333</v>
+        <v>0.93</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>5</v>
@@ -491,10 +491,10 @@
         <v>0.001</v>
       </c>
       <c r="B3" s="5">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="C3" s="5">
-        <v>80</v>
+        <v>0.8</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -512,10 +512,10 @@
         <v>0.1</v>
       </c>
       <c r="B4" s="5">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="C4" s="5">
-        <v>73.33</v>
+        <v>0.73</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -533,10 +533,10 @@
         <v>0.316</v>
       </c>
       <c r="B5" s="5">
-        <v>95.5555555555556</v>
+        <v>0.96</v>
       </c>
       <c r="C5" s="5">
-        <v>46.67</v>
+        <v>0.47</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -554,10 +554,10 @@
         <v>1</v>
       </c>
       <c r="B6" s="5">
-        <v>93.3333333333333</v>
+        <v>0.93</v>
       </c>
       <c r="C6" s="5">
-        <v>26.67</v>
+        <v>0.27</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -575,7 +575,7 @@
         <v>3.16</v>
       </c>
       <c r="B7" s="5">
-        <v>20</v>
+        <v>0.2</v>
       </c>
       <c r="C7" s="5">
         <v>0</v>

</xml_diff>